<commit_message>
preparação de perguntas LLM
</commit_message>
<xml_diff>
--- a/docs/explanation/Juris-TCU-query-generation.xlsx
+++ b/docs/explanation/Juris-TCU-query-generation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Documents\GitHub\ind-ir\docs\explanation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5EBC1B-51A9-4AC2-A685-CDBD88CA89AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABFB1B1-9F81-4D0F-A5A7-72974009AC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{BF1A5944-88C4-44F0-AA41-0038DECDCCDF}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{BF1A5944-88C4-44F0-AA41-0038DECDCCDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries - a partir do log" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
   <si>
     <t>técnica e preço</t>
   </si>
@@ -304,13 +304,449 @@
   </si>
   <si>
     <t>Geração de QRELS para a base JURIS-TCU por LLM</t>
+  </si>
+  <si>
+    <t>#44162
+Os serviços técnicos necessários à estruturação de projeto de parceria público-privada relativo à modernização, eficientização, expansão, operação e manutenção da infraestrutura de rede de iluminação pública são, em regra, serviços comuns, licitados na modalidade de pregão.</t>
+  </si>
+  <si>
+    <t>Qual é a modalidade de licitação utilizada para contratar serviços técnicos necessários à estruturação de projeto de parceria público-privada relativo a infraestrutura de rede de iluminação pública?</t>
+  </si>
+  <si>
+    <t>projeto de parceria público-privada modalidade</t>
+  </si>
+  <si>
+    <t>* Prompt utilizado "Elabore até 5 perguntas curtas e diretas que possam ser respondidas a partir do enunciado a seguir: /n/n{texto_enunciado}"</t>
+  </si>
+  <si>
+    <t>#13694
+Para fins de habilitação jurídica nas licitações, faz-se necessária a compatibilidade entre o objeto do certame e as atividades previstas no contrato social das empresas licitantes.</t>
+  </si>
+  <si>
+    <t>O que acontece se não houver compatibilidade entre o objeto do certame e as atividades previstas no contrato social da empresa licitante?</t>
+  </si>
+  <si>
+    <t>objeto do certame contrato social licitante</t>
+  </si>
+  <si>
+    <t>#13583
+A responsabilidade pela gestão dos recursos do Fundo Municipal de Saúde é do secretário de saúde (art. 9º, inciso III, da Lei 8.080/1990) . Independentemente da participação de outros agentes na prática de determinados atos de administração dos recursos, remanesce para o secretário a responsabilidade primeira pela correta aplicação dos recursos e pelo alcance dos objetivos estabelecidos no Sistema Único de Saúde.</t>
+  </si>
+  <si>
+    <t>Quem é responsável pela gestão dos recursos do Fundo Municipal de Saúde?</t>
+  </si>
+  <si>
+    <t>responsabilidade gestão dos recursos Fundo Municipal de Saúde</t>
+  </si>
+  <si>
+    <t>#31629
+Quando da elaboração do orçamento-base da licitação, deve ser realizada ampla pesquisa de mercado para a formação dos preços orçados, utilizando-se de fontes oficiais ou de orçamentos emitidos por, no mínimo, três fornecedores, quando houver, a qual deverá necessariamente estar documentada no processo licitatório.</t>
+  </si>
+  <si>
+    <t>É obrigatória pesquisa de mercado na elaboração do orçamento-base da licitação?</t>
+  </si>
+  <si>
+    <t>pesquisa de mercado orçamento fornecedores</t>
+  </si>
+  <si>
+    <t>#52912
+A mera comparação dos valores constantes em ata de registro de preços com os obtidos junto a empresas consultadas na fase interna de licitação não é suficiente para configurar a vantajosidade da adesão à ata, haja vista que os preços informados nas consultas, por vezes superestimados, não serão, em regra, os efetivamente contratados. Deve o órgão não participante ("carona") , com o intuito de aferir a adequação dos preços praticados na ata, se socorrer de outras fontes, a exemplo de licitações e contratos similares realizados no âmbito da Administração Pública.</t>
+  </si>
+  <si>
+    <t>O que fazer para verificar a vantajosidade da adesão à ata?</t>
+  </si>
+  <si>
+    <t>vantajosidade adesão à ata</t>
+  </si>
+  <si>
+    <t>#10089
+Como regra geral, para atendimento dos limites definidos no art. 65, §§ 1º e 2º, da Lei 8.666/1993, os acréscimos ou supressões nos montantes dos contratos firmados pelos órgãos e entidades da Administração Pública devem ser considerados de forma isolada, sendo calculados sobre o valor original do contrato, vedada a compensação entre acréscimos e supressões.</t>
+  </si>
+  <si>
+    <t>#134594
+As reduções ou supressões de quantitativos decorrentes de alteração contratual devem ser consideradas de forma isolada, ou seja, o conjunto de reduções e o conjunto de acréscimos devem ser sempre calculados sobre o valor original do contrato, aplicando-se a cada um desses conjuntos, individualmente e sem nenhum tipo de compensação entre eles, os limites de alteração estabelecidos no art. 65, § 1º, da Lei 8.666/1993.</t>
+  </si>
+  <si>
+    <t>É permitida a compensação entre acréscimos e supressões nos contratos administrativos?</t>
+  </si>
+  <si>
+    <t>compensação entre acréscimos e supressões contratos administrativos</t>
+  </si>
+  <si>
+    <t>#34132
+Em licitações para aquisição de tonalizadores e cartuchos de tinta para impressoras ou outros produtos análogos, a Administração deve evitar a indicação de preferência por marcas, ante a falta de amparo legal, salvo na hipótese em que fique demonstrado tecnicamente que só determinada marca atenderá à necessidade da Administração, situação devidamente justificada e demonstrada no processo.</t>
+  </si>
+  <si>
+    <t>#13633
+Não se admite, como regra, a especificação de marca para aquisição de cartuchos para impressoras. No entanto, o Tribunal aceita esse tipo de exigência quando os equipamentos em que os cartuchos serão utilizados estiverem em período de garantia e os termos de garantia previrem que ela somente se aplicará caso os produtos neles utilizados forem originais.</t>
+  </si>
+  <si>
+    <t>A Administração pode indicar preferência por marcas em licitações para aquisição de cartuchos de tinta?</t>
+  </si>
+  <si>
+    <t>marca aquisição cartuchos</t>
+  </si>
+  <si>
+    <t>#13553
+Os recursos repassados pela União, no âmbito do Sistema Único de Saúde, aos estados, ao Distrito Federal e aos municípios constituem recursos federais. Estão sujeitos à fiscalização do TCU as ações e os serviços de saúde pagos à conta desses recursos, quer sejam transferidos mediante convênio, quer sejam repassados com base em outro instrumento ou ato legal.</t>
+  </si>
+  <si>
+    <t>O TCU é responsável pela fiscalização das ações e serviços de saúde pagos com recursos repassados pela União no âmbito do Sistema Único de Saúde?</t>
+  </si>
+  <si>
+    <t>SUS recursos União competência do TCU</t>
+  </si>
+  <si>
+    <t>#22165
+No caso de não ser possível obter preços referenciais nos sistemas oficiais para a estimativa de custos em processos licitatórios, deve ser realizada pesquisa de preços contendo o mínimo de três cotações de empresas/fornecedores distintos, fazendo constar do respectivo processo a documentação comprobatória pertinente aos levantamentos e estudos que fundamentaram o preço estimado. Caso não seja possível obter esse número de cotações, deve ser elaborada justificativa circunstanciada.</t>
+  </si>
+  <si>
+    <t>O que deve ser feito se não for possível obter preços referenciais nos sistemas oficiais para estimativa de custos em processos licitatórios?</t>
+  </si>
+  <si>
+    <t>preços referenciais sistemas oficiais estimativa de custos</t>
+  </si>
+  <si>
+    <t>#21159
+A adoção, em licitação do tipo técnica e preço, de peso excessivamente elevado para a pontuação técnica em relação à de preço, sem justificativa plausível, e de critérios subjetivos de julgamento das propostas contraria o disposto nos arts. 3º, 40, inciso VII, 44, § 1º, e 45, da Lei 8.666/1993.</t>
+  </si>
+  <si>
+    <t>É necessária ponderação entre a pontuação técnica e a de preço em uma licitação do tipo técnica e preço?</t>
+  </si>
+  <si>
+    <t>ponderação técnica e preço</t>
+  </si>
+  <si>
+    <t>#21229
+O estabelecimento de critério de pontuação técnica, em licitação do tipo técnica e preço, que valoriza excessivamente determinado quesito, em detrimento do preço, restringe o caráter competitivo do certame e compromete a obtenção da proposta mais vantajosa para a Administração.</t>
+  </si>
+  <si>
+    <t>Qual é o impacto de valorizar excessivamente um quesito na licitação do tipo técnica e preço?</t>
+  </si>
+  <si>
+    <t>#133563
+Em licitações do tipo técnica e preço, o edital deve definir critérios objetivos para a gradação das notas a serem dadas a cada quesito da avaliação técnica, assim como distribuir a pontuação técnica de modo proporcional à relevância de cada quesito para a execução do objeto contratual, de forma a permitir o julgamento objetivo das propostas e evitar o estabelecimento de pontuação desarrazoada, limitadora da competitividade.</t>
+  </si>
+  <si>
+    <t>Como a pontuação desarrazoada pode limitar a competitividade nas licitações do tipo técnica e preço?</t>
+  </si>
+  <si>
+    <t>pontuação desarrazoada licitações técnica e preço</t>
+  </si>
+  <si>
+    <t>#693
+Em regra a prorrogação do contrato administrativo deve ser efetuada antes do término do prazo de vigência, mediante termo aditivo, para que não se opere a extinção do ajuste. Entretanto, excepcionalmente e para evitar prejuízo ao interesse público, nos contratos de escopo, diante da inércia do agente em formalizar tempestivamente o devido aditamento, é possível considerar os períodos de paralisação das obras por iniciativa da Administração contratante como períodos de suspensão da contagem do prazo de vigência do ajuste.</t>
+  </si>
+  <si>
+    <t>É possível prorrogar um contrato administrativo fora do término do prazo de vigência?</t>
+  </si>
+  <si>
+    <t>prorrogação de contrato administrativo término prazo de vigência</t>
+  </si>
+  <si>
+    <t>#105994
+Na contratação de serviços advocatícios por conselho de fiscalização profissional, é excessiva a exigência de apresentação de atestado de capacidade técnica emitido por pessoa jurídica de conselho de classe, pois não se vislumbra, como regra, a necessidade de expertise na prestação de serviços jurídicos a tais entidades.</t>
+  </si>
+  <si>
+    <t>Qual é o problema na exigência de atestado de capacidade técnica para contratação de serviços advocatícios por conselho de fiscalização profissional?</t>
+  </si>
+  <si>
+    <t>atestado de capacidade técnica serviços advocatícios conselho de fiscalização profissional</t>
+  </si>
+  <si>
+    <t>#29832
+É dispensável a reposição de importâncias indevidamente percebidas, de boa-fé, por servidores ativos e inativos, e pensionistas, em virtude de erro escusável de interpretação de lei por parte do órgão/entidade.</t>
+  </si>
+  <si>
+    <t>É necessária reposição de importâncias indevidamente percebidas, de boa-fé, por servidores, em virtude de erro escusável de interpretação de lei por parte do órgão/entidade?</t>
+  </si>
+  <si>
+    <t>reposição de importâncias indevidamente percebidas boa-fé servidores erro escusável por órgão/entidade</t>
+  </si>
+  <si>
+    <t>#17105
+O dano reverso decorrente da falta de produto ou serviço que possa colocar em risco a saúde de pessoas se mostra muito mais gravoso do que o potencial dano ao erário decorrente da aquisição direta para remediar a situação, não podendo ser cobrada do gestor a prática de conduta diversa.</t>
+  </si>
+  <si>
+    <t>É possível aquisição direta quando a falta de produto ou serviço pode colocar em risco a saúde das pessoas?</t>
+  </si>
+  <si>
+    <t>aquisição direta risco a saúde</t>
+  </si>
+  <si>
+    <t>#71456
+Nos pregões para aquisição de medicamentos, a divulgação dos preços estimados da contratação no edital do certame prejudica a obtenção da proposta mais vantajosa para a Administração.</t>
+  </si>
+  <si>
+    <t>É obrigatória a divulgação dos preços estimados no edital nos pregões para aquisição de medicamentos?</t>
+  </si>
+  <si>
+    <t>pregão divulgação dos preços estimados no edital</t>
+  </si>
+  <si>
+    <t>#31507
+As contratações de professores, conferencistas ou instrutores para ministrar cursos de treinamento ou aperfeiçoamento de pessoal enquadram-se na hipótese de inexigibilidade de licitação prevista no inciso II do art. 25, combinado com o inciso VI do art. 13 da Lei 8.666/1993.</t>
+  </si>
+  <si>
+    <t>A contratação de professores, conferencistas ou instrutores para ministrar cursos de treinamento ou aperfeiçoamento de pessoal se enquadra na inexigibilidade de licitação?</t>
+  </si>
+  <si>
+    <t>instrutor treinamento inexigibilidade de licitação</t>
+  </si>
+  <si>
+    <t>#31108
+Reequilíbrio econômico é o reestabelecimento da relação contratual inicialmente ajustada pelas partes, por conta da ocorrência de álea extraordinária, superveniente ao originalmente contratado. O reajuste de preços é a reposição da perda do poder aquisitivo da moeda por meio do emprego de índices de preços prefixados no contrato administrativo. A repactuação, referente a contratos de serviços contínuos, ocorre a partir da variação dos componentes dos custos do contrato, devendo ser demonstrada analiticamente, de acordo com a Planilha de Custos e Formação de Preços.</t>
+  </si>
+  <si>
+    <t>#31104
+A diferença entre repactuação e reajuste é que este é automático e realizado periodicamente, mediante aplicação de índice de preço que, dentro do possível, deve refletir os custos setoriais. Enquanto que naquela, de periodicidade anual, não há automatismo, pois é necessário demonstrar a variação dos custos do serviço. Para que ocorra a repactuação, com base na variação dos custos do serviço contratado, deve ser observado o prazo mínimo de um ano, mediante a demonstração analítica da variação dos componentes dos custos, devidamente justificada, não sendo admissível repactuação com base na variação do IGPM.</t>
+  </si>
+  <si>
+    <t>Qual é a diferença entre reajuste de preços e repactuação?</t>
+  </si>
+  <si>
+    <t>reajuste de preços e repactuação</t>
+  </si>
+  <si>
+    <t>#42820
+Ainda que a Administração tenha aplicado o reajuste previsto no contrato, justifica-se a aplicação da recomposição sempre que se verificar a presença de seus pressupostos, uma vez que o reajuste e a recomposição possuem fundamentos distintos. O reajuste, previsto nos arts. 40, inciso XI, e 55, inciso III, da Lei 8.666/1993, visa remediar os efeitos da inflação. A recomposição, prevista no art. 65, inciso II, alínea d, da Lei 8.666/1993, tem como fim manter equilibrada a relação jurídica entre o particular e a Administração Pública quando houver desequilíbrio advindo de fato imprevisível ou previsível com consequências incalculáveis.</t>
+  </si>
+  <si>
+    <t>É possível a aplicação da recomposição mesmo após a aplicação do reajuste previsto no contrato?</t>
+  </si>
+  <si>
+    <t>recomposição reajuste</t>
+  </si>
+  <si>
+    <t>#17220
+A perda da regularidade fiscal, inclusive quanto à seguridade social, no curso de contratos de execução continuada ou parcelada justifica a imposição de sanções à contratada, mas não autoriza a retenção de pagamentos por serviços prestados.</t>
+  </si>
+  <si>
+    <t>A retenção de pagamentos é permitida em caso de perda da regularidade fiscal?</t>
+  </si>
+  <si>
+    <t>retenção de pagamentos perda da regularidade fiscal</t>
+  </si>
+  <si>
+    <t>#104455
+O restabelecimento total ou parcial de quantitativo de item anteriormente suprimido por aditivo contratual amparado no art. 65, §§ 1º e 2º, da Lei 8.666/1993, em razão de restrições orçamentárias, desde que observadas as mesmas condições e preços iniciais pactuados, não configura a compensação vedada pela jurisprudência do TCU, consubstanciada nos &lt;acordao_decisao_tcu colegiado="Plenário" numero="1536" ano="2016" &gt;acórdãos 1.536/2016-Plenário&lt;/acordao_decisao_tcu&gt; e 2.554/2017-Plenário, visto que o objeto licitado fica inalterado, sendo possível, portanto, além do restabelecimento, novos acréscimos sobre o valor original do contrato, observados os limites estabelecidos no art. 65, § 1º, da Lei 8.666/1993.não configura a compensação vedada pela jurisprudência do TCU, consubstanciada nos &lt;acordao_decisao_tcu colegiado="Plenário" numero="1536" ano="2016" &gt;acórdãos 1.536/2016-Plenário&lt;/acordao_decisao_tcu&gt; e 2.554/2017-Plenário, visto que o objeto licitado fica inalterado, sendo possível, portanto, além do restabelecimento, novos acréscimos sobre o valor original do contrato, observados os limites estabelecidos no art. 65, § 1º, da Lei 8.666/1993.</t>
+  </si>
+  <si>
+    <t>Quais são as condições para que o restabelecimento total ou parcial de quantitativo de item anteriormente suprimido por aditivo contratual não configure compensação vedada pela jurisprudência do TCU?</t>
+  </si>
+  <si>
+    <t>vedado restabelecimento item suprimido</t>
+  </si>
+  <si>
+    <t>#33081
+São irregulares os quesitos de pontuação técnica para cujo atendimento as empresas licitantes tenham de incorrer em despesas que sejam desnecessárias e anteriores à celebração do contrato ou frustrem o caráter competitivo do certame, a exemplo da pontuação para licitantes que possuírem, já na abertura da licitação, determinado quadro de pessoal com técnicos certificados e qualificados; a existência de plataforma de treinamento à distância para os funcionários da licitante; ambiente próprio de help desk para suporte remoto aos profissionais do contrato.</t>
+  </si>
+  <si>
+    <t>Por que despesas desnecessárias e anteriores à celebração do contrato são consideradas irregulares?</t>
+  </si>
+  <si>
+    <t>irregulares despesas desnecessárias e anteriores à celebração do contrato</t>
+  </si>
+  <si>
+    <t>#22841
+A exigência de quadro de pessoal técnico pré-existente e ligado à licitante por vínculo trabalhista ou societário privilegia empresas de grande porte e levam as licitantes a efetuar despesas com a contratação de pessoal simplesmente com a finalidade de participar do certame licitatório.</t>
+  </si>
+  <si>
+    <t>Como o vínculo trabalhista ou societário pré-existente afeta a competitividade das licitantes no certame licitatório?</t>
+  </si>
+  <si>
+    <t>vínculo trabalhista ou societário pré-existente competitividade das licitantes</t>
+  </si>
+  <si>
+    <t>#43098
+É irregular, nas licitações de técnica e preço, atribuir pontuação para empresa licitante simplesmente por possuir, em seu quadro permanente, por determinado tempo, certos tipos de profissionais, o que pode vir a inibir o caráter competitivo do certame e privilegiar empresas de grande porte, além de não garantir que os mesmos profissionais sejam alocados na execução do objeto.</t>
+  </si>
+  <si>
+    <t>É permitido atribuir pontuação a uma empresa licitante nas licitações de técnica e preço com base na posse de determinados tipos de profissionais em seu quadro permanente?</t>
+  </si>
+  <si>
+    <t>técnica e preço profissionais quadro permanente</t>
+  </si>
+  <si>
+    <t>#85586
+A mera existência de erro material ou de omissão na planilha de custos e de formação de preços da licitante não enseja, necessariamente, a desclassificação antecipada da sua proposta, devendo a Administração promover diligência junto ao interessado para a correção das falhas, sem permitir, contudo, a alteração do valor global originalmente proposto.</t>
+  </si>
+  <si>
+    <t>Um erro material deve levar à desclassificação antecipada da proposta?</t>
+  </si>
+  <si>
+    <t>erro material desclassificação da proposta</t>
+  </si>
+  <si>
+    <t>#122028
+A vedação à inclusão de novo documento, prevista no art. 43, § 3º, da Lei 8.666/1993 e no art. 64 da Lei 14.133/2021 (nova Lei de Licitações e Contratos Administrativos) , não alcança documento destinado a atestar condição de habilitação preexistente à abertura da sessão pública, apresentado em sede de diligência.</t>
+  </si>
+  <si>
+    <t>Há vedação à inclusão de novo documento destinado a atestar condição de habilitação preexistente em sede de diligência?</t>
+  </si>
+  <si>
+    <t>vedação à inclusão documento habilitação diligência</t>
+  </si>
+  <si>
+    <t>#21864
+É obrigatória, nos processos de licitação, dispensa ou inexigibilidade, a consulta dos preços correntes no mercado, dos fixados por órgão oficial competente ou, ainda, dos constantes em sistema de registro de preços. A ausência de pesquisa de preços configura descumprimento de exigência legal.</t>
+  </si>
+  <si>
+    <t>A pesquisa de preços correntes no mercado é obrigatória em licitações?</t>
+  </si>
+  <si>
+    <t>pesquisa de preços obrigatória em licitações</t>
+  </si>
+  <si>
+    <t>#22780
+SÚMULA TCU 263: Para a comprovação da capacidade técnico-operacional das licitantes, e desde que limitada, simultaneamente, às parcelas de maior relevância e valor significativo do objeto a ser contratado, é legal a exigência de comprovação da execução de quantitativos mínimos em obras ou serviços com características semelhantes, devendo essa exigência guardar proporção com a dimensão e a complexidade do objeto a ser executado.</t>
+  </si>
+  <si>
+    <t>A exigência de comprovação de quantitativos mínimos em obras ou serviços com características semelhantes é legal?</t>
+  </si>
+  <si>
+    <t>exigência comprovação de quantitativos mínimos características semelhantes</t>
+  </si>
+  <si>
+    <t>#98454
+Os efeitos da sanção de impedimento de licitar e contratar prevista no art. 7º da Lei 10.520/2002 se estendem a toda a esfera de governo do órgão ou da entidade que aplicou a penalidade, incluindo as empresas estatais.</t>
+  </si>
+  <si>
+    <t>Qual a extensão da sanção de impedimento de licitar e contratar?</t>
+  </si>
+  <si>
+    <t>extensão sanção de impedimento de licitar e contratar</t>
+  </si>
+  <si>
+    <t>#79794
+Para fins de habilitação técnico-operacional em certames visando à contratação de obras e serviços de engenharia, devem ser exigidos atestados emitidos em nome da licitante, podendo ser solicitadas as certidões de acervo técnico (CAT) ou anotações/registros de responsabilidade técnica (ART/RRT) emitidas pelo conselho de fiscalização profissional competente em nome dos profissionais vinculados aos referidos atestados, como forma de conferir autenticidade e veracidade às informações constantes nos documentos emitidos em nome das licitantes.</t>
+  </si>
+  <si>
+    <t>Quais documentos são exigidos para habilitação técnico-operacional em certames de obras e serviços de engenharia?</t>
+  </si>
+  <si>
+    <t>habilitação técnico-operacional obras e serviços de engenharia</t>
+  </si>
+  <si>
+    <t>#110879
+Cabe ao órgão gerenciador da ata de registro de preços o controle das autorizações de adesão, a fim de que os quantitativos de cada item registrado contratados pelos caronas não superem os limites previstos no art. 22, §§ 3º, 4º e 4º-A, do Decreto 7.892/2013.</t>
+  </si>
+  <si>
+    <t>Qual a finalidade do controle das autorizações de adesão?</t>
+  </si>
+  <si>
+    <t>controle adesão</t>
+  </si>
+  <si>
+    <t>#45379
+Para fins de habilitação jurídica, é vedada a exigência de apresentação de alvará de funcionamento sem a demonstração de que o documento constitui exigência do Poder Público para o funcionamento da licitante, o que deve ser evidenciado mediante indicação expressa da norma de regência no edital da licitação.</t>
+  </si>
+  <si>
+    <t>Em que situações a apresentação do alvará de funcionamento é permitida na habilitação jurídica?</t>
+  </si>
+  <si>
+    <t>alvará de funcionamento habilitação jurídica</t>
+  </si>
+  <si>
+    <t>#20797
+O cargo de secretário municipal, por ter natureza política, não pode ser considerado cargo técnico ou científico, pois não exige o domínio de conhecimentos especializados. Contudo, é regular sua acumulação com o cargo de professor, se neste o servidor estiver em licença para tratar de interesse particular, não se aplicando a Súmula 246 do TCU.</t>
+  </si>
+  <si>
+    <t>É permitida a acumulação do cargo de secretário municipal com o cargo de professor?</t>
+  </si>
+  <si>
+    <t>acumulação de cargo secretário municipal professor</t>
+  </si>
+  <si>
+    <t>#135564
+Em processo de prestação ou tomada de contas ordinária ou extraordinária, a inexistência de débito e a simultânea prescrição da pretensão punitiva do TCU não impedem o julgamento pela irregularidade das contas.</t>
+  </si>
+  <si>
+    <t>A prescrição da pretensão punitiva do TCU afeta o julgamento das contas?</t>
+  </si>
+  <si>
+    <t>prescrição da pretensão punitiva julgamento das contas</t>
+  </si>
+  <si>
+    <t>#86727
+É válida a utilização do Banco de Preços em Saúde do Ministério da Saúde (BPS) como referência de preços para aquisição de medicamentos e, consequentemente, para fins de quantificação de superfaturamento e sobrepreço, desde que balizada por critérios adequados, que aproximem a pesquisa à contratação analisada.</t>
+  </si>
+  <si>
+    <t>O Banco de Preços em Saúde é uma referência de preços válida para a aquisição de medicamentos?</t>
+  </si>
+  <si>
+    <t>Banco de Preços em Saúde referência medicamentos</t>
+  </si>
+  <si>
+    <t>#147727
+A mera comparação dos valores constantes em ata de registro de preços com os obtidos junto a empresas consultadas na fase interna de licitação não é suficiente para configurar a vantajosidade da adesão à ata, haja vista que os preços informados nas consultas, por vezes superestimados, não serão, em regra, os efetivamente contratados. Deve o órgão não participante ("carona") , com o intuito de aferir a adequação dos preços praticados na ata, se socorrer de outras fontes, a exemplo de licitações e contratos similares realizados no âmbito da Administração Pública.</t>
+  </si>
+  <si>
+    <t>#72668
+É irregular alteração contratual para incluir, no instrumento pactuado, serviços já previstos no edital como obrigação da futura contratada, mas que foram omitidos na planilha orçamentária da obra. Só se admite alteração, quantitativa ou qualitativa, decorrente de fato superveniente à celebração do contrato, e desde que haja interesse público no aditamento.</t>
+  </si>
+  <si>
+    <t>É possível a inclusão de serviços já previstos no edital em uma alteração contratual</t>
+  </si>
+  <si>
+    <t>alteração contratual serviços já previstos no edital</t>
+  </si>
+  <si>
+    <t>#452
+A observância das normas e das disposições do edital, consoante o art. 41, caput, da Lei 8.666/93, deve ser aplicada mediante a consideração dos princípios basilares que norteiam o procedimento licitatório, dentre eles os da eficiência e da seleção da proposta mais vantajosa. Diante do caso concreto, e a fim de melhor viabilizar a concretização do interesse público, pode o princípio da legalidade estrita ser afastado frente a outros princípios.</t>
+  </si>
+  <si>
+    <t>O princípio da legalidade estrita pode ser afastado em favor de outros princípios no procedimento licitatório?</t>
+  </si>
+  <si>
+    <t>licitação princípio da legalidade estrita afastado</t>
+  </si>
+  <si>
+    <t>#43880
+Na demonstração da vantajosidade de eventual renovação de contrato de serviços de natureza continuada, deve ser realizada ampla pesquisa de preços, priorizando-se consultas a portais de compras governamentais e a contratações similares de outros entes públicos, utilizando-se apenas subsidiariamente a pesquisa com fornecedores.</t>
+  </si>
+  <si>
+    <t>Quais fontes devem ser prioritárias na pesquisa de preços para a renovação do contrato de serviços de natureza continuada?</t>
+  </si>
+  <si>
+    <t>renovação de contrato serviços de natureza continuada pesquisa de preços</t>
+  </si>
+  <si>
+    <t>#64928
+Nas contratações de &lt;i&gt;software&lt;/i&gt; fundadas no art. 25, inciso I, da Lei 8.666/1993, não devem ser aceitas cartas de exclusividade emitidas pelos próprios fabricantes, porquanto são válidos apenas os atestados emitidos pelos entes mencionados no referido dispositivo.</t>
+  </si>
+  <si>
+    <t>Devem ser aceitas nas contratações de software as cartas de exclusividade emitidas pelos próprios fabricantes?</t>
+  </si>
+  <si>
+    <t>contratações de software cartas de exclusividade</t>
+  </si>
+  <si>
+    <t>#17892
+A contratação de entidade para prestação de serviços de assistência médica a servidores deve, em regra, ser precedida de licitação, sob pena de afronta ao disposto no art. 2º da Lei 8.666/1993.</t>
+  </si>
+  <si>
+    <t>Qual é a regra geral para a contratação de entidade para prestação de serviços de assistência médica a servidores?</t>
+  </si>
+  <si>
+    <t>assistência médica a servidores</t>
+  </si>
+  <si>
+    <t>#129357
+A exigência de comprovação da execução de quantitativos mínimos em obras ou serviços com características semelhantes, para fins de atestar a capacidade técnico-operacional, deve guardar proporção com a dimensão e a complexidade do objeto e recair, simultaneamente, sobre as parcelas de maior relevância e valor significativo. Como regra, os quantitativos mínimos exigidos não devem ultrapassar 50% do previsto no orçamento base, salvo em condições especiais e devidamente justificadas no processo de licitação.simultaneamente, sobre as parcelas de maior relevância e valor significativo. Como regra, os quantitativos mínimos exigidos não devem ultrapassar 50% do previsto no orçamento base, salvo em condições especiais e devidamente justificadas no processo de licitação.</t>
+  </si>
+  <si>
+    <t>Quais critérios devem ser considerados ao exigir comprovação da execução de quantitativos mínimos em obras ou serviços?</t>
+  </si>
+  <si>
+    <t>comprovação quantitativos mínimos obras serviços</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,16 +770,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF343541"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -366,11 +814,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -381,19 +857,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCD"/>
+      <color rgb="FFFFFF9B"/>
+      <color rgb="FFFFFF3B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4925,7 +5427,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="pt-BR"/>
-            <a:t>Geração de prompt</a:t>
+            <a:t>Geração de prompt*</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -8461,7 +8963,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>Geração de prompt</a:t>
+            <a:t>Geração de prompt*</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -9842,8 +10344,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="729512" y="0"/>
-          <a:ext cx="3393139" cy="2221230"/>
+          <a:off x="744469" y="0"/>
+          <a:ext cx="3384408" cy="2215515"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -9914,8 +10416,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1577797" y="333185"/>
-        <a:ext cx="1767424" cy="1554861"/>
+        <a:off x="1590571" y="332327"/>
+        <a:ext cx="1762876" cy="1550861"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{95D39365-8A21-4033-8750-3FC7497DED78}">
@@ -9925,8 +10427,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="329685" y="475343"/>
-          <a:ext cx="1270543" cy="1270543"/>
+          <a:off x="345670" y="474120"/>
+          <a:ext cx="1267274" cy="1267274"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -9992,8 +10494,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="515752" y="661410"/>
-        <a:ext cx="898409" cy="898409"/>
+        <a:off x="531258" y="659708"/>
+        <a:ext cx="896098" cy="896098"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F29B0C26-01A1-42F6-90A5-51D99F1EA160}">
@@ -10003,8 +10505,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4567256" y="0"/>
-          <a:ext cx="4207913" cy="2221230"/>
+          <a:off x="4572825" y="0"/>
+          <a:ext cx="4197086" cy="2215515"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -10093,8 +10595,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5619234" y="333185"/>
-        <a:ext cx="2378504" cy="1554861"/>
+        <a:off x="5622096" y="332327"/>
+        <a:ext cx="2372385" cy="1550861"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{13A4D77D-F8D7-4C34-A595-C387D1AC2406}">
@@ -10104,8 +10606,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4298422" y="475343"/>
-          <a:ext cx="1270543" cy="1270543"/>
+          <a:off x="4304682" y="474120"/>
+          <a:ext cx="1267274" cy="1267274"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -10183,8 +10685,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4484489" y="661410"/>
-        <a:ext cx="898409" cy="898409"/>
+        <a:off x="4490270" y="659708"/>
+        <a:ext cx="896098" cy="896098"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{370F8907-19B4-430A-8163-2C42FCD88B7B}">
@@ -10194,8 +10696,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="9111676" y="0"/>
-          <a:ext cx="2541087" cy="2221230"/>
+          <a:off x="9106039" y="0"/>
+          <a:ext cx="2534549" cy="2215515"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -10231,8 +10733,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="8943926" y="475343"/>
-          <a:ext cx="1270543" cy="1270543"/>
+          <a:off x="8938720" y="474120"/>
+          <a:ext cx="1267274" cy="1267274"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -10298,8 +10800,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="9129993" y="661410"/>
-        <a:ext cx="898409" cy="898409"/>
+        <a:off x="9124308" y="659708"/>
+        <a:ext cx="896098" cy="896098"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -15624,13 +16126,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15683,13 +16185,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>518159</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15742,13 +16244,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>34290</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15778,14 +16280,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>120016</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133257</xdr:rowOff>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137067</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -15839,13 +16341,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15875,13 +16377,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>87629</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>97154</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>39911</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -16432,7 +16934,7 @@
   <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16697,11 +17199,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EF176E-4EC8-4CFA-A20A-A271E5EC1BC0}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16725,10 +17225,10 @@
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -16736,17 +17236,17 @@
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -16754,10 +17254,10 @@
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -16765,10 +17265,10 @@
       <c r="A6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -16776,10 +17276,10 @@
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -16787,10 +17287,10 @@
       <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -16798,10 +17298,10 @@
       <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -16809,10 +17309,10 @@
       <c r="A10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -16820,117 +17320,588 @@
       <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>171</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+    <row r="21" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+    <row r="29" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+    <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+    <row r="31" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="str">
+        <f>_xlfn.CONCAT("Quantidade de enunciados:   ",COUNTA(A2:A57))</f>
+        <v>Quantidade de enunciados:   56</v>
+      </c>
+      <c r="B58" s="13" t="str">
+        <f>_xlfn.CONCAT("Quantidade de perguntas:   ",COUNTA(B2:B57))</f>
+        <v>Quantidade de perguntas:   51</v>
+      </c>
+      <c r="C58" s="13" t="str">
+        <f>_xlfn.CONCAT("Quant. expressões de busca:   ",COUNTA(C2:C57))</f>
+        <v>Quant. expressões de busca:   50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="11">
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16939,77 +17910,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCEE529-1188-454F-9B3B-AB4BF4AFF475}">
-  <dimension ref="B5:AB27"/>
+  <dimension ref="B2:AB39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="7" t="s">
+    <row r="2" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
     </row>
-    <row r="27" spans="2:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B27" s="7" t="s">
+    <row r="21" spans="2:28" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+    </row>
+    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B39" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B5:V5"/>
-    <mergeCell ref="B27:AB27"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="B21:AB21"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17017,67 +17994,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3A8440-71DE-41B2-A5FA-3EB22ACB81E7}">
   <dimension ref="B5:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
     </row>
     <row r="27" spans="2:28" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="8"/>
-      <c r="AB27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -17090,6 +18067,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c54ba682-435e-47ec-8b13-e8a29c78a21b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D35DEDE583B66F4CADF9255F0166439D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1734d530a3629da431b6c81c4441fa0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c54ba682-435e-47ec-8b13-e8a29c78a21b" xmlns:ns4="ad60b73e-940f-4d9b-9be1-93ac2919cec6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbbbe93fc951698c00aa3177733bc481" ns3:_="" ns4:_="">
     <xsd:import namespace="c54ba682-435e-47ec-8b13-e8a29c78a21b"/>
@@ -17324,24 +18318,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98563E12-44D7-4DD2-ACAA-E11CDCDE276F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ad60b73e-940f-4d9b-9be1-93ac2919cec6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c54ba682-435e-47ec-8b13-e8a29c78a21b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c54ba682-435e-47ec-8b13-e8a29c78a21b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C731428-5691-4D3F-8A33-9B33DCAA73A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4E94FB6-5DA5-40AF-9D7A-C87F8215D13D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17358,29 +18360,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C731428-5691-4D3F-8A33-9B33DCAA73A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98563E12-44D7-4DD2-ACAA-E11CDCDE276F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ad60b73e-940f-4d9b-9be1-93ac2919cec6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c54ba682-435e-47ec-8b13-e8a29c78a21b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>